<commit_message>
Code cleanup, better Obstacles numeration
</commit_message>
<xml_diff>
--- a/WZORY/LISTA PRZESZKÓD.xlsx
+++ b/WZORY/LISTA PRZESZKÓD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48530\PyCharmProjects\RMG-Tables\WZORY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F974243-95FE-40A7-86AD-5F48F4BE0705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DAA432-65DD-4BEE-AEF7-4E07F2A8B7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1662,7 +1662,7 @@
   </sheetPr>
   <dimension ref="A1:X1048470"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>

</xml_diff>